<commit_message>
änderungen aus google drive
</commit_message>
<xml_diff>
--- a/helper_skripts/menu_converter/menu-2024.08.09.xlsx
+++ b/helper_skripts/menu_converter/menu-2024.08.09.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Local/benefi/helper_skripts/menu_converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2F4FB0-1E32-BB4E-BD7E-17F6DD823B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98912E2-DB01-9742-B390-E3775F6ACDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{66CE5546-DD97-6C42-971C-9AA23625C39F}"/>
   </bookViews>
@@ -1474,9 +1474,9 @@
   </sheetPr>
   <dimension ref="A1:I165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1912,9 +1912,7 @@
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="2">
-        <v>9</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="4" t="s">
         <v>9</v>
       </c>
@@ -3579,7 +3577,7 @@
       <c r="F109" s="14"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3">
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="I109" s="3"/>
     </row>
@@ -3697,7 +3695,7 @@
       <c r="F115" s="14"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="I115" s="3"/>
     </row>
@@ -4394,7 +4392,7 @@
       <c r="F150" s="14"/>
       <c r="G150" s="3"/>
       <c r="H150" s="3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I150" s="3"/>
     </row>
@@ -4413,7 +4411,7 @@
       <c r="F151" s="14"/>
       <c r="G151" s="3"/>
       <c r="H151" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I151" s="3"/>
     </row>

</xml_diff>